<commit_message>
added ability to try find invisible buttons after initial finding visible buttons failed.
</commit_message>
<xml_diff>
--- a/Websites.xlsx
+++ b/Websites.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
   <si>
     <t>instructables.com</t>
   </si>
@@ -85,12 +85,6 @@
   </si>
   <si>
     <t>hulu.com</t>
-  </si>
-  <si>
-    <t>Good?</t>
-  </si>
-  <si>
-    <t>bad</t>
   </si>
   <si>
     <t>http://www.squidoo.com/</t>
@@ -290,17 +284,20 @@
   <si>
     <t>need to agree to user agreement</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cannot detect login button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -308,13 +305,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -351,8 +348,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -365,7 +362,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -439,6 +436,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -473,6 +471,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -648,24 +647,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="1"/>
-    <col min="8" max="8" width="51.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="36.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -685,10 +684,10 @@
         <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -707,9 +706,6 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
@@ -756,10 +752,10 @@
         <v>4</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -776,7 +772,7 @@
         <v>18</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -792,13 +788,10 @@
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -810,7 +803,7 @@
         <v>4</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -821,422 +814,422 @@
         <v>16</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H72" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I72" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1250,12 +1243,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1263,12 +1256,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bug fixed: squidoo.com phase 14, error.
</commit_message>
<xml_diff>
--- a/Websites.xlsx
+++ b/Websites.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="93">
   <si>
     <t>instructables.com</t>
   </si>
@@ -287,17 +287,29 @@
   </si>
   <si>
     <t>Cannot detect login button</t>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vul</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>token</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -305,13 +317,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -348,8 +360,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -362,7 +374,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -436,7 +448,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -471,7 +482,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -647,24 +657,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="36.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -706,6 +716,9 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
@@ -720,6 +733,9 @@
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
@@ -788,6 +804,9 @@
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
@@ -801,6 +820,9 @@
       </c>
       <c r="D8" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>88</v>
@@ -1243,12 +1265,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1256,12 +1278,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
to eliminate lots of 'follow us on facebook' buttons, we add weight to buttons having login/signin pattern.
</commit_message>
<xml_diff>
--- a/Websites.xlsx
+++ b/Websites.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="94">
   <si>
     <t>instructables.com</t>
   </si>
@@ -299,17 +299,20 @@
   <si>
     <t>token</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>popup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -317,13 +320,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -360,8 +363,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -374,7 +377,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -448,6 +451,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -482,6 +486,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -657,24 +662,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="36.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -835,7 +840,35 @@
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="H9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -845,22 +878,6 @@
       </c>
       <c r="H24" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1265,12 +1282,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1278,12 +1295,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
minor changes to xlsx.
</commit_message>
<xml_diff>
--- a/Websites.xlsx
+++ b/Websites.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
   <si>
     <t>instructables.com</t>
   </si>
@@ -24,16 +24,10 @@
     <t>Homepage</t>
   </si>
   <si>
-    <t>Callback</t>
-  </si>
-  <si>
     <t>Auth form</t>
   </si>
   <si>
     <t>Popup</t>
-  </si>
-  <si>
-    <t>set cookie + refresh page</t>
   </si>
   <si>
     <t>answers.com</t>
@@ -311,6 +305,15 @@
   </si>
   <si>
     <t>popup, and then click</t>
+  </si>
+  <si>
+    <t>IdP</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -684,636 +687,649 @@
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>96</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>91</v>
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>91</v>
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
+      <c r="H4" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>90</v>
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>92</v>
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="I12" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="I13" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="I14" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="I15" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="3" customFormat="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="3" customFormat="1">
       <c r="A27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="3" customFormat="1">
+        <v>28</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1">
       <c r="A28" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>94</v>
+        <v>32</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>87</v>
+        <v>42</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>29</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>29</v>
+        <v>62</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>29</v>
+        <v>66</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>29</v>
+        <v>67</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>29</v>
+        <v>68</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>29</v>
+        <v>69</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>29</v>
+        <v>70</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>29</v>
+        <v>72</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H72" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>29</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>31</v>
+        <v>78</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>29</v>
+        <v>79</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>29</v>
+        <v>81</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
major revision: added search for second/third best button, flickr still has navigation issues, didnt test invisible/total fail scnearios.
</commit_message>
<xml_diff>
--- a/Websites.xlsx
+++ b/Websites.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="117">
   <si>
     <t>instructables.com</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Login Button position</t>
   </si>
   <si>
-    <t>Login button form</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>netflix.com</t>
   </si>
   <si>
-    <t>Additionals</t>
-  </si>
-  <si>
     <t>Only having a netflix account first and then link it works.</t>
   </si>
   <si>
@@ -274,13 +268,6 @@
   </si>
   <si>
     <t>requires linking</t>
-  </si>
-  <si>
-    <t>need to agree to user agreement</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cannot detect login button</t>
   </si>
   <si>
     <t>code</t>
@@ -314,6 +301,75 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>registration style</t>
+  </si>
+  <si>
+    <t>Login button</t>
+  </si>
+  <si>
+    <t>layer, form</t>
+  </si>
+  <si>
+    <t>redirection, form</t>
+  </si>
+  <si>
+    <t>redirection, a</t>
+  </si>
+  <si>
+    <t>layer, input</t>
+  </si>
+  <si>
+    <t>submit button</t>
+  </si>
+  <si>
+    <t>hard - see explain</t>
+  </si>
+  <si>
+    <t>extra</t>
+  </si>
+  <si>
+    <t>registration?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Y/no info needed</t>
+  </si>
+  <si>
+    <t>detect login button</t>
+  </si>
+  <si>
+    <t>Embed the layer in https, not accessible by SOP</t>
+  </si>
+  <si>
+    <t>a/img</t>
+  </si>
+  <si>
+    <t>a/a</t>
+  </si>
+  <si>
+    <t>a/div</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>div/a</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>a/span</t>
+  </si>
+  <si>
+    <t>a paragraph discribing fb is detected, instead of the real thing.</t>
+  </si>
+  <si>
+    <t>weird - navigation problems</t>
   </si>
 </sst>
 </file>
@@ -371,7 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,6 +436,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -684,53 +743,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>103</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,19 +808,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -758,578 +831,659 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="I5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>104</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>105</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>104</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="4" customFormat="1">
+      <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
+      <c r="F26" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="4" customFormat="1">
+      <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1" t="s">
+      <c r="F27" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="3" customFormat="1">
-      <c r="A27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1">
-      <c r="A28" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="F28" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I34" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="1" t="s">
-        <v>37</v>
+      <c r="F29" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I53" s="1" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I59" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I60" s="1" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>29</v>
+        <v>77</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I77" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I78" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="1" t="s">
-        <v>84</v>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
confirmed invisible and fail cases.
</commit_message>
<xml_diff>
--- a/Websites.xlsx
+++ b/Websites.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="118">
   <si>
     <t>instructables.com</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>weird - navigation problems</t>
+  </si>
+  <si>
+    <t>invisible button</t>
   </si>
 </sst>
 </file>
@@ -746,7 +749,7 @@
   <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1082,6 +1085,9 @@
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
fixed two bugs on deciding login button clicking correctness.
</commit_message>
<xml_diff>
--- a/Websites.xlsx
+++ b/Websites.xlsx
@@ -366,13 +366,13 @@
     <t>a/span</t>
   </si>
   <si>
-    <t>a paragraph discribing fb is detected, instead of the real thing.</t>
-  </si>
-  <si>
-    <t>weird - navigation problems</t>
-  </si>
-  <si>
     <t>invisible button</t>
+  </si>
+  <si>
+    <t>a/div (3rd highest)</t>
+  </si>
+  <si>
+    <t>weird navigation problems, doesn't happen all the time</t>
   </si>
 </sst>
 </file>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1087,7 +1087,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>113</v>
@@ -1121,7 +1121,7 @@
         <v>109</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1132,6 +1132,25 @@
         <v>108</v>
       </c>
     </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="26" spans="1:10" s="4" customFormat="1">
       <c r="A26" s="4" t="s">
         <v>26</v>
@@ -1163,25 +1182,6 @@
       </c>
       <c r="J28" s="1" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:9">

</xml_diff>

<commit_message>
extend login button search to input element, fixed a try catch bug.
</commit_message>
<xml_diff>
--- a/Websites.xlsx
+++ b/Websites.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="122">
   <si>
     <t>instructables.com</t>
   </si>
@@ -373,6 +373,18 @@
   </si>
   <si>
     <t>weird navigation problems, doesn't happen all the time</t>
+  </si>
+  <si>
+    <t>Not vul</t>
+  </si>
+  <si>
+    <t>input!</t>
+  </si>
+  <si>
+    <t>Detect login status</t>
+  </si>
+  <si>
+    <t>Problem</t>
   </si>
 </sst>
 </file>
@@ -746,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -757,18 +769,19 @@
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="40.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
         <v>91</v>
       </c>
@@ -785,25 +798,28 @@
         <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -819,14 +835,14 @@
       <c r="F2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -842,14 +858,14 @@
       <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -865,14 +881,14 @@
       <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -891,14 +907,14 @@
       <c r="F5" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -914,14 +930,14 @@
       <c r="F6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -937,11 +953,11 @@
       <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -957,20 +973,20 @@
       <c r="F8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -983,14 +999,14 @@
       <c r="F9" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1006,14 +1022,14 @@
       <c r="F10" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -1029,14 +1045,14 @@
       <c r="F11" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1049,14 +1065,14 @@
       <c r="F12" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1069,14 +1085,14 @@
       <c r="F13" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1092,14 +1108,14 @@
       <c r="F14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1107,7 +1123,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1120,7 +1136,7 @@
       <c r="F16" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1139,7 +1155,8 @@
       <c r="F18" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="G18" s="4"/>
+      <c r="J18" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1147,349 +1164,367 @@
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="4" customFormat="1">
-      <c r="A26" s="4" t="s">
+      <c r="J19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" s="4" customFormat="1">
+      <c r="A74" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F74" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" s="4" customFormat="1">
-      <c r="A27" s="4" t="s">
+      <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="1:11" s="4" customFormat="1">
+      <c r="A75" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F75" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="1" t="s">
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F76" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J28" s="1" t="s">
+      <c r="G76" s="3"/>
+      <c r="J76" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K76" s="1" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
-      <c r="A77" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed a bug of login detection
</commit_message>
<xml_diff>
--- a/Websites.xlsx
+++ b/Websites.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="120">
   <si>
     <t>instructables.com</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>ask.com</t>
-  </si>
-  <si>
-    <t>import info</t>
   </si>
   <si>
     <t>imdb.com</t>
@@ -285,12 +282,6 @@
     <t>popup</t>
   </si>
   <si>
-    <t>Bad, reason: the login element located is not 'a', clicking its parent node/children would help</t>
-  </si>
-  <si>
-    <t>Bad, reason: string doesn't have login pattern, just have FB</t>
-  </si>
-  <si>
     <t>popup, and then click</t>
   </si>
   <si>
@@ -342,9 +333,6 @@
     <t>detect login button</t>
   </si>
   <si>
-    <t>Embed the layer in https, not accessible by SOP</t>
-  </si>
-  <si>
     <t>a/img</t>
   </si>
   <si>
@@ -384,7 +372,13 @@
     <t>Detect login status</t>
   </si>
   <si>
-    <t>Problem</t>
+    <t>Problem(outerhtml doesn't match)</t>
+  </si>
+  <si>
+    <t>SOP</t>
+  </si>
+  <si>
+    <t>Y, also does linking</t>
   </si>
 </sst>
 </file>
@@ -758,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -783,40 +777,40 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -833,13 +827,13 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -859,10 +853,10 @@
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -885,7 +879,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -893,7 +887,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -905,13 +899,13 @@
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -928,13 +922,13 @@
         <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -954,7 +948,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -971,19 +965,19 @@
         <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -997,13 +991,13 @@
         <v>3</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1017,16 +1011,16 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1040,439 +1034,424 @@
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="4" customFormat="1">
+      <c r="A14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G18" s="4"/>
       <c r="J18" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J47" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J65" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="J65" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -1485,46 +1464,59 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" s="4" customFormat="1">
-      <c r="A74" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G74" s="3"/>
+        <v>82</v>
+      </c>
     </row>
     <row r="75" spans="1:11" s="4" customFormat="1">
       <c r="A75" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G75" s="3"/>
+        <v>118</v>
+      </c>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G76" s="3"/>
+        <v>118</v>
+      </c>
+      <c r="G76" s="4"/>
       <c r="J76" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>